<commit_message>
Update data in backend
</commit_message>
<xml_diff>
--- a/backend/data.xlsx
+++ b/backend/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -609,9 +609,37 @@
         <v>24/8/2025, 12:19:11 pm</v>
       </c>
     </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>rfṭy</v>
+      </c>
+      <c r="B16" t="str">
+        <v>tydty@gmail.com</v>
+      </c>
+      <c r="C16" t="str">
+        <v>cyctfg6 4</v>
+      </c>
+      <c r="D16" t="str">
+        <v>26/8/2025, 5:43:17 pm</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>rfṭy</v>
+      </c>
+      <c r="B17" t="str">
+        <v>tydty@gmail.com</v>
+      </c>
+      <c r="C17" t="str">
+        <v>cyctfg6 4</v>
+      </c>
+      <c r="D17" t="str">
+        <v>26/8/2025, 5:43:22 pm</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>